<commit_message>
Tuneado el lector de xlsx
</commit_message>
<xml_diff>
--- a/assets/reporteCursos.xlsx
+++ b/assets/reporteCursos.xlsx
@@ -3582,35 +3582,35 @@
   <dimension ref="A1:AI394"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="52.3805668016194"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="52.3805668016194"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="30" min="27" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="10.6032388663968"/>
   </cols>

</xml_diff>

<commit_message>
Funcion parsea excel hace update y create
</commit_message>
<xml_diff>
--- a/assets/reporteCursos.xlsx
+++ b/assets/reporteCursos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6824" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6841" uniqueCount="1144">
   <si>
     <t>Listado de Cursos</t>
   </si>
@@ -3446,6 +3446,12 @@
   </si>
   <si>
     <t>THE PRACTICE OF EVERYDAY LIFE</t>
+  </si>
+  <si>
+    <t>DESTRONCADA DE CHOTA</t>
+  </si>
+  <si>
+    <t>07-03-2017</t>
   </si>
 </sst>
 </file>
@@ -3579,38 +3585,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI394"/>
+  <dimension ref="A1:AI395"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A379" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C391" activeCellId="0" sqref="C391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5222672064777"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="54.5222672064777"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="54.5222672064777"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="30" min="27" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="10.6032388663968"/>
   </cols>
@@ -4325,7 +4331,7 @@
         <v>79</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="T8" s="0" t="s">
         <v>80</v>
@@ -43702,7 +43708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
         <v>1140</v>
       </c>
@@ -43798,6 +43804,104 @@
       </c>
       <c r="AH394" s="4" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A395" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B395" s="3" t="n">
+        <v>19098</v>
+      </c>
+      <c r="C395" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D395" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E395" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F395" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="G395" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="H395" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I395" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J395" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="K395" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L395" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="M395" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N395" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O395" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="P395" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q395" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="T395" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="U395" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="V395" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="W395" s="3" t="n">
+        <v>114</v>
+      </c>
+      <c r="X395" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y395" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z395" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA395" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB395" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC395" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD395" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE395" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF395" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG395" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH395" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejorado la carga de archivos
</commit_message>
<xml_diff>
--- a/assets/reporteCursos.xlsx
+++ b/assets/reporteCursos.xlsx
@@ -3448,7 +3448,7 @@
     <t xml:space="preserve">THE PRACTICE OF EVERYDAY LIFE</t>
   </si>
   <si>
-    <t xml:space="preserve">DESTRONCADA DE CHOTA v2</t>
+    <t xml:space="preserve">prueba de cambio v2</t>
   </si>
   <si>
     <t xml:space="preserve">07-03-2017</t>
@@ -3594,28 +3594,28 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="55.0607287449393"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="20" min="19" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="30" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="10.6032388663968"/>

</xml_diff>

<commit_message>
corregido texto user test
</commit_message>
<xml_diff>
--- a/assets/reporteCursos.xlsx
+++ b/assets/reporteCursos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -3463,7 +3463,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -3487,14 +3487,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <u val="single"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3564,7 +3556,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3587,38 +3579,38 @@
   </sheetPr>
   <dimension ref="A1:AI395"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A379" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C395" activeCellId="0" sqref="C395"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="30" min="27" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="10.6032388663968"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="9" style="0" width="56.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="56.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="56.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="56.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="27" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="10.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43910,7 +43902,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>